<commit_message>
finalizing first data cleaning
</commit_message>
<xml_diff>
--- a/modelisation_files/etat_batiment.xlsx
+++ b/modelisation_files/etat_batiment.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>E000086</t>
+          <t>E000048</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>E000353</t>
+          <t>E000239</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,19 +472,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E000358</t>
+          <t>E000249</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>E000164</t>
+          <t>E000179</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,19 +496,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>E000337</t>
+          <t>E000360</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>E000029</t>
+          <t>E000334</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>E000120</t>
+          <t>E000187</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E000347</t>
+          <t>E000273</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>E000178</t>
+          <t>E000107</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>E000114</t>
+          <t>E000124</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,31 +568,31 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>E000188</t>
+          <t>E000076</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>E000327</t>
+          <t>E000070</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>E000222</t>
+          <t>E000266</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,67 +604,67 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>E000047</t>
+          <t>E000177</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>E000179</t>
+          <t>E000174</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>E000257</t>
+          <t>E000090</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>E000316</t>
+          <t>E000004</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>E000302</t>
+          <t>E000292</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>E000340</t>
+          <t>E000200</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>E000083</t>
+          <t>E000254</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,19 +688,19 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>E000266</t>
+          <t>E000029</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>E000351</t>
+          <t>E000075</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>E000214</t>
+          <t>E000135</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -724,19 +724,19 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>E000373</t>
+          <t>E000022</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>E000040</t>
+          <t>E000104</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>E000335</t>
+          <t>E000291</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>E000063</t>
+          <t>E000117</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -772,19 +772,19 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>E000342</t>
+          <t>E000260</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>E000056</t>
+          <t>E000019</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>E000064</t>
+          <t>E000238</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,31 +808,31 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>E000339</t>
+          <t>E000327</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>E000217</t>
+          <t>E000108</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>E000054</t>
+          <t>E000005</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -844,19 +844,19 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>E000239</t>
+          <t>E000315</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>E000035</t>
+          <t>E000159</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>E000299</t>
+          <t>E000247</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -880,55 +880,55 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>E000008</t>
+          <t>E000195</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>E000085</t>
+          <t>E000313</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>E000268</t>
+          <t>E000148</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>E000036</t>
+          <t>E000366</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>E000156</t>
+          <t>E000017</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -940,7 +940,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>E000211</t>
+          <t>E000018</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>E000300</t>
+          <t>E000199</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -964,19 +964,19 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>E000258</t>
+          <t>E000335</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>E000270</t>
+          <t>E000307</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -988,31 +988,31 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>E000057</t>
+          <t>E000267</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>E000252</t>
+          <t>E000231</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>E000171</t>
+          <t>E000044</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>E000108</t>
+          <t>E000184</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1036,7 +1036,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>E000281</t>
+          <t>E000204</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>E000189</t>
+          <t>E000351</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1060,31 +1060,31 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>E000019</t>
+          <t>E000222</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>E000110</t>
+          <t>E000329</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>E000167</t>
+          <t>E000155</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>E000289</t>
+          <t>E000002</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>E000304</t>
+          <t>E000034</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1120,19 +1120,19 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>E000144</t>
+          <t>E000173</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>E000096</t>
+          <t>E000040</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1144,7 +1144,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>E000192</t>
+          <t>E000210</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>E000343</t>
+          <t>E000028</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>E000194</t>
+          <t>E000381</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>E000134</t>
+          <t>E000082</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>E000282</t>
+          <t>E000167</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1204,43 +1204,43 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>E000366</t>
+          <t>E000279</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>E000379</t>
+          <t>E000343</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>E000209</t>
+          <t>E000346</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>E000344</t>
+          <t>E000180</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>E000135</t>
+          <t>E000272</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1264,7 +1264,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>E000014</t>
+          <t>E000056</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1276,7 +1276,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>E000041</t>
+          <t>E000121</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1288,19 +1288,19 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>E000303</t>
+          <t>E000024</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>E000272</t>
+          <t>E000338</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1312,7 +1312,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>E000323</t>
+          <t>E000217</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>E000099</t>
+          <t>E000113</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -1336,31 +1336,31 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>E000363</t>
+          <t>E000099</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>E000317</t>
+          <t>E000324</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>E000017</t>
+          <t>E000213</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1372,19 +1372,19 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>E000365</t>
+          <t>E000074</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>E000294</t>
+          <t>E000262</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1396,7 +1396,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>E000360</t>
+          <t>E000322</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -1408,7 +1408,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>E000210</t>
+          <t>E000096</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -1420,7 +1420,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>E000137</t>
+          <t>E000116</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -1432,7 +1432,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>E000066</t>
+          <t>E000036</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1444,19 +1444,19 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>E000042</t>
+          <t>E000367</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>E000091</t>
+          <t>E000201</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1468,55 +1468,55 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>E000184</t>
+          <t>E000299</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>E000380</t>
+          <t>E000337</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>E000275</t>
+          <t>E000234</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>E000013</t>
+          <t>E000359</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>E000334</t>
+          <t>E000050</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -1528,7 +1528,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>E000136</t>
+          <t>E000282</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -1540,7 +1540,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>E000378</t>
+          <t>E000358</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -1552,7 +1552,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>E000081</t>
+          <t>E000285</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -1564,7 +1564,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>E000200</t>
+          <t>E000276</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>E000016</t>
+          <t>E000233</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -1588,7 +1588,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>E000191</t>
+          <t>E000309</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -1600,19 +1600,19 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>E000279</t>
+          <t>E000176</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>E000312</t>
+          <t>E000250</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -1624,7 +1624,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>E000117</t>
+          <t>E000077</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -1636,31 +1636,31 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>E000174</t>
+          <t>E000191</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>E000269</t>
+          <t>E000144</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>E000181</t>
+          <t>E000119</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -1672,55 +1672,55 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>E000127</t>
+          <t>E000059</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>E000355</t>
+          <t>E000326</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>E000112</t>
+          <t>E000240</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>E000228</t>
+          <t>E000318</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>E000133</t>
+          <t>E000066</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -1732,7 +1732,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>E000130</t>
+          <t>E000020</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -1744,31 +1744,31 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>E000098</t>
+          <t>E000162</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>E000004</t>
+          <t>E000302</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>E000307</t>
+          <t>E000118</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -1780,7 +1780,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>E000050</t>
+          <t>E000033</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -1792,31 +1792,31 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>E000183</t>
+          <t>E000165</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>E000361</t>
+          <t>E000319</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>E000207</t>
+          <t>E000209</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -1828,7 +1828,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>E000115</t>
+          <t>E000189</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -1840,7 +1840,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>E000078</t>
+          <t>E000264</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -1852,7 +1852,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>E000321</t>
+          <t>E000105</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -1864,7 +1864,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>E000213</t>
+          <t>E000061</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -1876,19 +1876,19 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>E000368</t>
+          <t>E000202</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>E000278</t>
+          <t>E000298</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -1900,7 +1900,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>E000277</t>
+          <t>E000296</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -1912,7 +1912,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>E000235</t>
+          <t>E000243</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -1924,7 +1924,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>E000295</t>
+          <t>E000220</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -1936,19 +1936,19 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>E000119</t>
+          <t>E000106</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>E000084</t>
+          <t>E000218</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -1960,7 +1960,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>E000250</t>
+          <t>E000350</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -1972,7 +1972,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>E000237</t>
+          <t>E000328</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -1984,7 +1984,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>E000381</t>
+          <t>E000274</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -1996,19 +1996,19 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>E000067</t>
+          <t>E000001</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>E000273</t>
+          <t>E000006</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -2020,31 +2020,31 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>E000229</t>
+          <t>E000054</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>E000377</t>
+          <t>E000265</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>E000169</t>
+          <t>E000010</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2056,7 +2056,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>E000009</t>
+          <t>E000261</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2068,7 +2068,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>E000216</t>
+          <t>E000057</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2080,19 +2080,19 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>E000185</t>
+          <t>E000253</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>E000046</t>
+          <t>E000133</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -2104,19 +2104,19 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>E000023</t>
+          <t>E000259</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>E000245</t>
+          <t>E000186</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -2128,7 +2128,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>E000001</t>
+          <t>E000281</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -2140,7 +2140,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>E000147</t>
+          <t>E000053</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -2152,7 +2152,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>E000159</t>
+          <t>E000021</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -2164,7 +2164,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>E000187</t>
+          <t>E000305</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -2176,7 +2176,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>E000027</t>
+          <t>E000352</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -2188,7 +2188,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>E000329</t>
+          <t>E000073</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -2200,7 +2200,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>E000202</t>
+          <t>E000332</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -2212,7 +2212,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>E000172</t>
+          <t>E000079</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -2224,19 +2224,19 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>E000284</t>
+          <t>E000371</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>E000215</t>
+          <t>E000277</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -2248,7 +2248,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>E000296</t>
+          <t>E000142</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -2260,7 +2260,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>E000070</t>
+          <t>E000115</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -2272,19 +2272,19 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>E000226</t>
+          <t>E000223</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>E000190</t>
+          <t>E000123</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -2296,19 +2296,19 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>E000253</t>
+          <t>E000227</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>E000052</t>
+          <t>E000232</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -2320,31 +2320,31 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>E000121</t>
+          <t>E000375</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>E000161</t>
+          <t>E000207</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>E000025</t>
+          <t>E000126</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -2356,7 +2356,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>E000231</t>
+          <t>E000051</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -2368,19 +2368,19 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>E000225</t>
+          <t>E000025</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>E000012</t>
+          <t>E000306</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -2392,7 +2392,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>E000280</t>
+          <t>E000286</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -2404,7 +2404,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>E000362</t>
+          <t>E000141</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -2416,7 +2416,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>E000031</t>
+          <t>E000038</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -2428,7 +2428,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>E000141</t>
+          <t>E000310</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -2440,7 +2440,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>E000205</t>
+          <t>E000132</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -2452,7 +2452,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>E000247</t>
+          <t>E000152</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -2464,19 +2464,19 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>E000372</t>
+          <t>E000256</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>E000212</t>
+          <t>E000311</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -2488,19 +2488,19 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>E000286</t>
+          <t>E000361</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>E000005</t>
+          <t>E000026</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -2512,7 +2512,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>E000301</t>
+          <t>E000146</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -2524,7 +2524,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>E000292</t>
+          <t>E000172</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -2536,19 +2536,19 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>E000346</t>
+          <t>E000171</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>E000034</t>
+          <t>E000357</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -2560,7 +2560,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>E000204</t>
+          <t>E000125</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -2572,7 +2572,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>E000093</t>
+          <t>E000045</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -2584,43 +2584,43 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>E000267</t>
+          <t>E000295</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>E000175</t>
+          <t>E000164</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>E000359</t>
+          <t>E000349</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>E000308</t>
+          <t>E000083</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -2632,31 +2632,31 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>E000313</t>
+          <t>E000252</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>E000357</t>
+          <t>E000374</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>E000077</t>
+          <t>E000011</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -2668,7 +2668,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>E000150</t>
+          <t>E000140</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -2680,7 +2680,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>E000116</t>
+          <t>E000015</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -2692,7 +2692,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>E000048</t>
+          <t>E000156</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -2704,7 +2704,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>E000246</t>
+          <t>E000221</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -2716,7 +2716,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>E000261</t>
+          <t>E000333</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -2728,7 +2728,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>E000291</t>
+          <t>E000246</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -2740,7 +2740,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>E000223</t>
+          <t>E000055</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -2752,7 +2752,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>E000100</t>
+          <t>E000347</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -2764,7 +2764,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>E000254</t>
+          <t>E000348</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -2776,19 +2776,19 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>E000283</t>
+          <t>E000160</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>E000236</t>
+          <t>E000288</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -2800,7 +2800,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>E000062</t>
+          <t>E000092</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -2812,7 +2812,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>E000153</t>
+          <t>E000120</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -2824,7 +2824,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>E000330</t>
+          <t>E000130</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -2836,7 +2836,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>E000082</t>
+          <t>E000362</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -2848,7 +2848,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>E000069</t>
+          <t>E000062</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -2860,7 +2860,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>E000206</t>
+          <t>E000237</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -2872,19 +2872,19 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>E000107</t>
+          <t>E000134</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>E000152</t>
+          <t>E000182</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -2896,7 +2896,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>E000290</t>
+          <t>E000013</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -2908,19 +2908,19 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>E000371</t>
+          <t>E000037</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>E000030</t>
+          <t>E000095</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -2932,7 +2932,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>E000331</t>
+          <t>E000215</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -2944,7 +2944,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>E000198</t>
+          <t>E000185</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -2956,7 +2956,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>E000122</t>
+          <t>E000269</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -2968,7 +2968,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>E000033</t>
+          <t>E000086</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -2980,7 +2980,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>E000352</t>
+          <t>E000345</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -2992,19 +2992,19 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>E000155</t>
+          <t>E000111</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>E000101</t>
+          <t>E000354</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -3016,7 +3016,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>E000326</t>
+          <t>E000372</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -3028,7 +3028,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>E000010</t>
+          <t>E000154</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -3040,7 +3040,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>E000146</t>
+          <t>E000183</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -3052,19 +3052,19 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>E000102</t>
+          <t>E000257</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>E000244</t>
+          <t>E000102</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -3076,31 +3076,31 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>E000370</t>
+          <t>E000114</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>E000162</t>
+          <t>E000363</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>E000350</t>
+          <t>E000087</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -3112,19 +3112,19 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>E000011</t>
+          <t>E000379</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>E000088</t>
+          <t>E000035</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -3136,55 +3136,55 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>E000104</t>
+          <t>E000112</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>E000163</t>
+          <t>E000380</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>E000306</t>
+          <t>E000369</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>E000160</t>
+          <t>E000271</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>E000305</t>
+          <t>E000030</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -3196,31 +3196,31 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>E000333</t>
+          <t>E000198</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>E000322</t>
+          <t>E000158</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>E000003</t>
+          <t>E000178</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -3232,7 +3232,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>E000238</t>
+          <t>E000065</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -3244,43 +3244,43 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>E000053</t>
+          <t>E000228</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>E000143</t>
+          <t>E000365</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>E000193</t>
+          <t>E000047</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>E000065</t>
+          <t>E000263</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -3292,7 +3292,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>E000123</t>
+          <t>E000041</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -3304,7 +3304,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>E000076</t>
+          <t>E000150</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -3316,31 +3316,31 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>E000182</t>
+          <t>E000303</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>E000154</t>
+          <t>E000194</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>E000073</t>
+          <t>E000242</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -3352,19 +3352,19 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>E000180</t>
+          <t>E000368</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>E000139</t>
+          <t>E000290</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -3376,7 +3376,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>E000234</t>
+          <t>E000336</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -3388,31 +3388,31 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>E000129</t>
+          <t>E000027</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>E000314</t>
+          <t>E000127</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>E000158</t>
+          <t>E000280</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -3424,7 +3424,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>E000024</t>
+          <t>E000071</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -3436,7 +3436,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>E000285</t>
+          <t>E000168</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -3448,7 +3448,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>E000242</t>
+          <t>E000206</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -3460,7 +3460,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>E000060</t>
+          <t>E000069</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -3472,7 +3472,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>E000142</t>
+          <t>E000093</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -3484,7 +3484,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>E000199</t>
+          <t>E000100</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -3496,7 +3496,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>E000186</t>
+          <t>E000007</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -3508,7 +3508,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>E000128</t>
+          <t>E000145</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -3520,7 +3520,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>E000055</t>
+          <t>E000248</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -3532,7 +3532,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>E000106</t>
+          <t>E000325</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -3544,19 +3544,19 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>E000148</t>
+          <t>E000225</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>E000220</t>
+          <t>E000251</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -3568,19 +3568,19 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>E000298</t>
+          <t>E000129</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>E000157</t>
+          <t>E000060</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -3592,7 +3592,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>E000038</t>
+          <t>E000224</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -3604,7 +3604,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>E000320</t>
+          <t>E000308</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -3616,7 +3616,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>E000218</t>
+          <t>E000009</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -3628,19 +3628,19 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>E000287</t>
+          <t>E000188</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>E000224</t>
+          <t>E000283</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -3652,7 +3652,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>E000097</t>
+          <t>E000103</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -3664,7 +3664,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>E000356</t>
+          <t>E000208</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -3676,7 +3676,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>E000232</t>
+          <t>E000355</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -3688,7 +3688,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>E000249</t>
+          <t>E000211</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -3700,19 +3700,19 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>E000259</t>
+          <t>E000255</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>E000240</t>
+          <t>E000330</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -3724,19 +3724,19 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>E000227</t>
+          <t>E000340</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>E000262</t>
+          <t>E000169</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -3748,19 +3748,19 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>E000075</t>
+          <t>E000275</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>E000079</t>
+          <t>E000143</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -3772,7 +3772,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>E000026</t>
+          <t>E000342</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -3784,7 +3784,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>E000271</t>
+          <t>E000122</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -3796,31 +3796,31 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>E000022</t>
+          <t>E000377</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>E000375</t>
+          <t>E000216</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>E000166</t>
+          <t>E000023</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -3832,19 +3832,19 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>E000297</t>
+          <t>E000128</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>E000051</t>
+          <t>E000278</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -3856,31 +3856,31 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>E000203</t>
+          <t>E000373</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>E000080</t>
+          <t>E000085</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>E000369</t>
+          <t>E000301</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -3892,31 +3892,31 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>E000274</t>
+          <t>E000153</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>E000332</t>
+          <t>E000109</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>E000255</t>
+          <t>E000078</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -3928,19 +3928,19 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>E000072</t>
+          <t>E000370</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>E000132</t>
+          <t>E000300</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -3952,7 +3952,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>E000094</t>
+          <t>E000147</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -3964,7 +3964,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>E000151</t>
+          <t>E000012</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -3976,7 +3976,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>E000219</t>
+          <t>E000072</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -3988,7 +3988,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>E000049</t>
+          <t>E000230</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -4000,7 +4000,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>E000318</t>
+          <t>E000314</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -4012,7 +4012,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>E000325</t>
+          <t>E000193</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -4024,7 +4024,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>E000103</t>
+          <t>E000097</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -4036,19 +4036,19 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>E000007</t>
+          <t>E000226</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>E000319</t>
+          <t>E000245</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -4060,19 +4060,19 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>E000374</t>
+          <t>E000049</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>E000221</t>
+          <t>E000244</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -4084,19 +4084,19 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>E000288</t>
+          <t>E000268</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>E000341</t>
+          <t>E000043</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -4108,7 +4108,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>E000230</t>
+          <t>E000157</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -4120,19 +4120,19 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>E000338</t>
+          <t>E000258</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>E000020</t>
+          <t>E000039</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -4144,43 +4144,43 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>E000196</t>
+          <t>E000016</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>E000043</t>
+          <t>E000161</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>E000195</t>
+          <t>E000008</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>E000131</t>
+          <t>E000344</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -4192,19 +4192,19 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>E000058</t>
+          <t>E000067</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>E000336</t>
+          <t>E000137</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -4216,7 +4216,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>E000071</t>
+          <t>E000068</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -4228,7 +4228,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>E000105</t>
+          <t>E000094</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -4240,31 +4240,31 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>E000265</t>
+          <t>E000175</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>E000111</t>
+          <t>E000031</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>E000324</t>
+          <t>E000192</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -4276,7 +4276,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>E000059</t>
+          <t>E000312</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -4288,7 +4288,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>E000126</t>
+          <t>E000136</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -4300,7 +4300,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>E000089</t>
+          <t>E000297</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -4312,19 +4312,19 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>E000243</t>
+          <t>E000197</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>E000328</t>
+          <t>E000058</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -4336,7 +4336,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>E000251</t>
+          <t>E000304</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -4348,19 +4348,19 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>E000074</t>
+          <t>E000376</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>E000264</t>
+          <t>E000219</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -4372,19 +4372,19 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>E000177</t>
+          <t>E000149</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>E000354</t>
+          <t>E000212</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -4396,19 +4396,19 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>E000256</t>
+          <t>E000003</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>E000138</t>
+          <t>E000287</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -4420,7 +4420,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>E000037</t>
+          <t>E000014</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -4432,19 +4432,19 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>E000367</t>
+          <t>E000181</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>E000068</t>
+          <t>E000205</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -4456,7 +4456,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>E000124</t>
+          <t>E000284</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -4468,7 +4468,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>E000345</t>
+          <t>E000270</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -4480,19 +4480,19 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>E000364</t>
+          <t>E000190</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>E000170</t>
+          <t>E000236</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -4504,7 +4504,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>E000039</t>
+          <t>E000170</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -4516,7 +4516,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>E000309</t>
+          <t>E000138</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -4528,7 +4528,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>E000293</t>
+          <t>E000317</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -4540,7 +4540,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>E000002</t>
+          <t>E000091</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -4552,7 +4552,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>E000044</t>
+          <t>E000084</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -4564,19 +4564,19 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>E000028</t>
+          <t>E000098</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>E000349</t>
+          <t>E000052</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -4588,7 +4588,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>E000095</t>
+          <t>E000320</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -4600,7 +4600,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>E000168</t>
+          <t>E000321</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -4612,7 +4612,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>E000201</t>
+          <t>E000323</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -4624,19 +4624,19 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>E000348</t>
+          <t>E000293</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>E000165</t>
+          <t>E000081</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -4648,19 +4648,19 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>E000260</t>
+          <t>E000341</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>E000263</t>
+          <t>E000339</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
@@ -4672,19 +4672,19 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>E000233</t>
+          <t>E000316</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>E000241</t>
+          <t>E000294</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -4696,7 +4696,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>E000140</t>
+          <t>E000356</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
@@ -4708,19 +4708,19 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>E000315</t>
+          <t>E000046</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>E000125</t>
+          <t>E000203</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -4732,7 +4732,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>E000276</t>
+          <t>E000131</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -4744,19 +4744,19 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>E000376</t>
+          <t>E000289</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>E000015</t>
+          <t>E000063</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -4768,7 +4768,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>E000092</t>
+          <t>E000353</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -4780,24 +4780,24 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>E000208</t>
+          <t>E000378</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>E000176</t>
+          <t>E000080</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
@@ -4816,7 +4816,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>E000173</t>
+          <t>E000331</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -4828,19 +4828,19 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>E000109</t>
+          <t>E000166</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>E000087</t>
+          <t>E000139</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -4852,19 +4852,19 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>E000145</t>
+          <t>E000101</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>E000310</t>
+          <t>E000089</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -4876,7 +4876,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>E000018</t>
+          <t>E000235</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -4888,19 +4888,19 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>E000045</t>
+          <t>E000229</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>E000311</t>
+          <t>E000042</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -4912,19 +4912,19 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>E000021</t>
+          <t>E000110</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>E000113</t>
+          <t>E000214</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -4936,31 +4936,31 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>E000090</t>
+          <t>E000364</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>E000197</t>
+          <t>E000088</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>to_repare</t>
+          <t>intact</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>E000006</t>
+          <t>E000241</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -4972,19 +4972,19 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>E000118</t>
+          <t>E000196</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>intact</t>
+          <t>to_repare</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>E000061</t>
+          <t>E000151</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -4996,7 +4996,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>E000248</t>
+          <t>E000163</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -5008,7 +5008,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>E000149</t>
+          <t>E000064</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">

</xml_diff>